<commit_message>
Final UI update before merging
</commit_message>
<xml_diff>
--- a/backend/reports/Daily_Report_2026-01-07.xlsx
+++ b/backend/reports/Daily_Report_2026-01-07.xlsx
@@ -475,10 +475,10 @@
         <v>263.27</v>
       </c>
       <c r="C2" t="n">
-        <v>262.31</v>
+        <v>261.33</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.36</v>
+        <v>-0.74</v>
       </c>
       <c r="E2" t="n">
         <v>32.46</v>
@@ -497,13 +497,13 @@
         <v>188.57</v>
       </c>
       <c r="C3" t="n">
-        <v>190.29</v>
+        <v>189.83</v>
       </c>
       <c r="D3" t="n">
-        <v>0.91</v>
+        <v>0.67</v>
       </c>
       <c r="E3" t="n">
-        <v>48.86</v>
+        <v>48.85</v>
       </c>
       <c r="F3" t="n">
         <v>-35.93</v>
@@ -519,13 +519,13 @@
         <v>479.56</v>
       </c>
       <c r="C4" t="n">
-        <v>487.7</v>
+        <v>488.38</v>
       </c>
       <c r="D4" t="n">
-        <v>1.7</v>
+        <v>1.84</v>
       </c>
       <c r="E4" t="n">
-        <v>24.37</v>
+        <v>24.38</v>
       </c>
       <c r="F4" t="n">
         <v>-20.56</v>
@@ -541,13 +541,13 @@
         <v>435.89</v>
       </c>
       <c r="C5" t="n">
-        <v>436.11</v>
+        <v>436.81</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05</v>
+        <v>0.21</v>
       </c>
       <c r="E5" t="n">
-        <v>62.79</v>
+        <v>62.8</v>
       </c>
       <c r="F5" t="n">
         <v>-48.19</v>
@@ -563,13 +563,13 @@
         <v>93707.14999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>91475.11</v>
+        <v>91122.69</v>
       </c>
       <c r="D6" t="n">
-        <v>-2.38</v>
+        <v>-2.76</v>
       </c>
       <c r="E6" t="n">
-        <v>34.52</v>
+        <v>34.54</v>
       </c>
       <c r="F6" t="n">
         <v>-32.15</v>

</xml_diff>